<commit_message>
Yeu cau chi tiet
</commit_message>
<xml_diff>
--- a/Plan-Quan-Ly-Ban-Quan-Ao.xlsx
+++ b/Plan-Quan-Ly-Ban-Quan-Ao.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NguyenDoQuocTuan\Desktop\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NguyenDoQuocTuan\Desktop\QuanLyBanQuanAo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -272,7 +272,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="165" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -323,14 +323,6 @@
       <sz val="16"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0" tint="-0.499984740745262"/>
-      <name val="Arial"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -446,7 +438,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -522,11 +514,8 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -999,11 +988,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-1113914144"/>
-        <c:axId val="-1113909792"/>
+        <c:axId val="-2035251536"/>
+        <c:axId val="-2035240656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1113914144"/>
+        <c:axId val="-2035251536"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1013,7 +1002,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1113909792"/>
+        <c:crossAx val="-2035240656"/>
         <c:crossesAt val="42544"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1021,7 +1010,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1113909792"/>
+        <c:axId val="-2035240656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42600"/>
@@ -1033,7 +1022,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1113914144"/>
+        <c:crossAx val="-2035251536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1410,7 +1399,7 @@
   <dimension ref="A2:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15"/>
@@ -1463,7 +1452,7 @@
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="30">
+      <c r="B7" s="29">
         <v>42609</v>
       </c>
       <c r="C7" s="1"/>
@@ -1472,7 +1461,7 @@
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="30">
+      <c r="B8" s="29">
         <v>42653</v>
       </c>
       <c r="C8" s="1"/>
@@ -1528,7 +1517,7 @@
         <f t="shared" ref="E12" si="0">D12-C12</f>
         <v>0</v>
       </c>
-      <c r="F12" s="31" t="s">
+      <c r="F12" s="30" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1549,7 +1538,7 @@
         <f t="shared" ref="E13:E27" si="1">D13-C13</f>
         <v>0</v>
       </c>
-      <c r="F13" s="31" t="s">
+      <c r="F13" s="30" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1570,8 +1559,8 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="F14" s="29" t="s">
-        <v>11</v>
+      <c r="F14" s="30" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="21.95" customHeight="1">

</xml_diff>

<commit_message>
Yeu cau ky thuat
</commit_message>
<xml_diff>
--- a/Plan-Quan-Ly-Ban-Quan-Ao.xlsx
+++ b/Plan-Quan-Ly-Ban-Quan-Ao.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NguyenDoQuocTuan\Desktop\QuanLyBanQuanAo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NguyenDoQuocTuan\Documents\GITHUB\QuanLyBanQuanAo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -237,9 +237,6 @@
     <t>Detailed Reqs.</t>
   </si>
   <si>
-    <t>Techincal Reqs.</t>
-  </si>
-  <si>
     <t>DB Development</t>
   </si>
   <si>
@@ -262,6 +259,9 @@
   </si>
   <si>
     <t>Completed</t>
+  </si>
+  <si>
+    <t>Technical Reqs.</t>
   </si>
 </sst>
 </file>
@@ -600,7 +600,7 @@
                   <c:v>Detailed Reqs.</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Techincal Reqs.</c:v>
+                  <c:v>Technical Reqs.</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>DB Development</c:v>
@@ -879,7 +879,7 @@
                   <c:v>Detailed Reqs.</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Techincal Reqs.</c:v>
+                  <c:v>Technical Reqs.</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>DB Development</c:v>
@@ -988,11 +988,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2035251536"/>
-        <c:axId val="-2035240656"/>
+        <c:axId val="1582432832"/>
+        <c:axId val="1582431200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2035251536"/>
+        <c:axId val="1582432832"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1002,7 +1002,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2035240656"/>
+        <c:crossAx val="1582431200"/>
         <c:crossesAt val="42544"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1010,7 +1010,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2035240656"/>
+        <c:axId val="1582431200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42600"/>
@@ -1022,7 +1022,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2035251536"/>
+        <c:crossAx val="1582432832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1399,7 +1399,7 @@
   <dimension ref="A2:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15"/>
@@ -1518,7 +1518,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="21.95" customHeight="1">
@@ -1539,7 +1539,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="21.95" customHeight="1">
@@ -1560,12 +1560,12 @@
         <v>3</v>
       </c>
       <c r="F14" s="30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="21.95" customHeight="1">
       <c r="A15" s="5" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>63</v>
@@ -1580,13 +1580,13 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>11</v>
+      <c r="F15" s="30" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="21.95" customHeight="1">
       <c r="A16" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>62</v>
@@ -1607,7 +1607,7 @@
     </row>
     <row r="17" spans="1:6" ht="21.95" customHeight="1">
       <c r="A17" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>62</v>
@@ -1628,7 +1628,7 @@
     </row>
     <row r="18" spans="1:6" ht="21.95" customHeight="1">
       <c r="A18" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>63</v>
@@ -1649,7 +1649,7 @@
     </row>
     <row r="19" spans="1:6" ht="21.95" customHeight="1">
       <c r="A19" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>63</v>
@@ -1691,7 +1691,7 @@
     </row>
     <row r="21" spans="1:6" ht="21.95" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>63</v>
@@ -1733,7 +1733,7 @@
     </row>
     <row r="23" spans="1:6" ht="21.95" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>62</v>
@@ -1796,7 +1796,7 @@
     </row>
     <row r="26" spans="1:6" ht="21.95" customHeight="1">
       <c r="A26" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>62</v>

</xml_diff>

<commit_message>
Co so du lieu
</commit_message>
<xml_diff>
--- a/Plan-Quan-Ly-Ban-Quan-Ao.xlsx
+++ b/Plan-Quan-Ly-Ban-Quan-Ao.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="77">
   <si>
     <t>Tasks</t>
   </si>
@@ -262,6 +262,9 @@
   </si>
   <si>
     <t>Technical Reqs.</t>
+  </si>
+  <si>
+    <t>In progress</t>
   </si>
 </sst>
 </file>
@@ -272,7 +275,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="165" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -329,6 +332,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -438,7 +449,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -516,6 +527,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -988,11 +1002,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="1582432832"/>
-        <c:axId val="1582431200"/>
+        <c:axId val="-528876416"/>
+        <c:axId val="-528878048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1582432832"/>
+        <c:axId val="-528876416"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1002,7 +1016,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1582431200"/>
+        <c:crossAx val="-528878048"/>
         <c:crossesAt val="42544"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1010,7 +1024,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1582431200"/>
+        <c:axId val="-528878048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42600"/>
@@ -1022,7 +1036,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1582432832"/>
+        <c:crossAx val="-528876416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1399,7 +1413,7 @@
   <dimension ref="A2:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15"/>
@@ -1601,8 +1615,8 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>11</v>
+      <c r="F16" s="31" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="21.95" customHeight="1">

</xml_diff>